<commit_message>
Closes #2: Upload de 2 ficheiros (Plasmids)
</commit_message>
<xml_diff>
--- a/1FXhRND7HAgtGgicinPEjvEGMtVt9KIZo0T8W_9JtOdU.xlsx
+++ b/1FXhRND7HAgtGgicinPEjvEGMtVt9KIZo0T8W_9JtOdU.xlsx
@@ -25,15 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="206">
   <si>
     <t>Applications</t>
   </si>
   <si>
     <t>reagents</t>
-  </si>
-  <si>
-    <t>labs</t>
   </si>
   <si>
     <t>Chemical</t>
@@ -225,13 +222,19 @@
     <t>plasmid_seq_primers</t>
   </si>
   <si>
-    <t>Sequence</t>
+    <t>Sequence 1</t>
   </si>
   <si>
     <t>plasmid_sequence</t>
   </si>
   <si>
     <t>File</t>
+  </si>
+  <si>
+    <t>Sequence 2</t>
+  </si>
+  <si>
+    <t>plasmid_sequence2</t>
   </si>
   <si>
     <t>Antibiotic resistance</t>
@@ -1153,9 +1156,7 @@
       </c>
     </row>
     <row r="3" ht="27.0" customHeight="1">
-      <c r="A3" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="A3" s="3"/>
     </row>
     <row r="4" ht="27.0" customHeight="1">
       <c r="B4" s="4"/>
@@ -2202,13 +2203,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="8"/>
@@ -2246,95 +2247,95 @@
     </row>
     <row r="3" ht="29.25" customHeight="1">
       <c r="A3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="D3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="E3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="F3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="G3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="H3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="I3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="J3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="K3" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="L3" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="M3" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="15" t="s">
+      <c r="N3" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="15" t="s">
+      <c r="O3" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="P3" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="P3" s="16" t="s">
+      <c r="Q3" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="Q3" s="16" t="s">
+      <c r="R3" s="16" t="s">
         <v>22</v>
-      </c>
-      <c r="R3" s="16" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="4" ht="29.25" customHeight="1">
       <c r="A4" s="26" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>26</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>27</v>
       </c>
       <c r="G4" s="29"/>
       <c r="H4" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I4" s="30"/>
       <c r="J4" s="31"/>
       <c r="K4" s="32"/>
       <c r="L4" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M4" s="9">
         <v>1.0</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P4" s="9"/>
       <c r="Q4" s="9"/>
@@ -2342,45 +2343,45 @@
     </row>
     <row r="5" ht="29.25" customHeight="1">
       <c r="A5" s="26" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5" s="9">
         <v>100.0</v>
       </c>
       <c r="G5" s="29"/>
       <c r="H5" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I5" s="30"/>
       <c r="J5" s="31"/>
       <c r="K5" s="32"/>
       <c r="L5" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M5" s="9">
         <v>2.0</v>
       </c>
       <c r="N5" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P5" s="9">
         <v>1.0</v>
       </c>
       <c r="Q5" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R5" s="9"/>
     </row>
@@ -2440,13 +2441,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="8"/>
@@ -2484,95 +2485,95 @@
     </row>
     <row r="3" ht="29.25" customHeight="1">
       <c r="A3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="D3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="E3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="F3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="G3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="H3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="I3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="J3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="K3" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="L3" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="M3" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="15" t="s">
+      <c r="N3" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="15" t="s">
+      <c r="O3" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="P3" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="P3" s="16" t="s">
+      <c r="Q3" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="Q3" s="16" t="s">
+      <c r="R3" s="16" t="s">
         <v>22</v>
-      </c>
-      <c r="R3" s="16" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="4" ht="29.25" customHeight="1">
       <c r="A4" s="26" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>26</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>27</v>
       </c>
       <c r="G4" s="29"/>
       <c r="H4" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I4" s="30"/>
       <c r="J4" s="31"/>
       <c r="K4" s="32"/>
       <c r="L4" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M4" s="9">
         <v>1.0</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P4" s="9"/>
       <c r="Q4" s="9"/>
@@ -2580,45 +2581,45 @@
     </row>
     <row r="5" ht="29.25" customHeight="1">
       <c r="A5" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>144</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>143</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5" s="9">
         <v>100.0</v>
       </c>
       <c r="G5" s="29"/>
       <c r="H5" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I5" s="30"/>
       <c r="J5" s="31"/>
       <c r="K5" s="32"/>
       <c r="L5" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M5" s="9">
         <v>2.0</v>
       </c>
       <c r="N5" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P5" s="9">
         <v>1.0</v>
       </c>
       <c r="Q5" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R5" s="9"/>
     </row>
@@ -2678,13 +2679,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C1" s="34" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="8"/>
@@ -2723,93 +2724,93 @@
     </row>
     <row r="3" ht="29.25" customHeight="1">
       <c r="A3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="D3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="E3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="F3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="G3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="H3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="I3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="J3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="K3" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="L3" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="M3" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="15" t="s">
+      <c r="N3" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="15" t="s">
+      <c r="O3" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="P3" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="P3" s="16" t="s">
+      <c r="Q3" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="Q3" s="16" t="s">
+      <c r="R3" s="16" t="s">
         <v>22</v>
-      </c>
-      <c r="R3" s="16" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="4" ht="29.25" customHeight="1">
       <c r="A4" s="17" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D4" s="18"/>
       <c r="E4" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="19" t="s">
         <v>26</v>
-      </c>
-      <c r="F4" s="19" t="s">
-        <v>27</v>
       </c>
       <c r="G4" s="20"/>
       <c r="H4" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I4" s="22"/>
       <c r="J4" s="22"/>
       <c r="K4" s="22"/>
       <c r="L4" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M4" s="19"/>
       <c r="N4" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O4" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P4" s="20"/>
       <c r="Q4" s="9"/>
@@ -2817,39 +2818,39 @@
     </row>
     <row r="5" ht="29.25" customHeight="1">
       <c r="A5" s="17" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D5" s="18"/>
       <c r="E5" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5" s="23">
         <v>100.0</v>
       </c>
       <c r="G5" s="20"/>
       <c r="H5" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I5" s="22"/>
       <c r="J5" s="22"/>
       <c r="K5" s="22"/>
       <c r="L5" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M5" s="23">
         <v>1.0</v>
       </c>
       <c r="N5" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O5" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P5" s="19">
         <v>1.0</v>
@@ -2908,46 +2909,46 @@
     <row r="1" ht="27.75" customHeight="1">
       <c r="A1" s="37"/>
       <c r="B1" s="38" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D1" s="40" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E1" s="40" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F1" s="40" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G1" s="40" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H1" s="40" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="I1" s="40" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="J1" s="40" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="K1" s="40" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="L1" s="40" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="M1" s="40" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="N1" s="40" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="O1" s="40" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="P1" s="41"/>
       <c r="Q1" s="41"/>
@@ -2960,16 +2961,16 @@
     </row>
     <row r="2" ht="27.75" customHeight="1">
       <c r="A2" s="42" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B2" s="43" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C2" s="44" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D2" s="44" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E2" s="45"/>
       <c r="F2" s="46"/>
@@ -2993,14 +2994,14 @@
     </row>
     <row r="3" ht="27.75" customHeight="1">
       <c r="A3" s="47" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B3" s="48"/>
       <c r="C3" s="49" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D3" s="49" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E3" s="50"/>
       <c r="F3" s="50"/>
@@ -3024,16 +3025,16 @@
     </row>
     <row r="4" ht="27.75" customHeight="1">
       <c r="A4" s="51" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B4" s="52" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C4" s="53" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D4" s="53" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E4" s="54"/>
       <c r="F4" s="54"/>
@@ -3057,14 +3058,14 @@
     </row>
     <row r="5" ht="27.75" customHeight="1">
       <c r="A5" s="47" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B5" s="48"/>
       <c r="C5" s="49" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" s="49" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E5" s="50"/>
       <c r="F5" s="50"/>
@@ -3088,19 +3089,19 @@
     </row>
     <row r="6" ht="27.75" customHeight="1">
       <c r="A6" s="51" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B6" s="52" t="s">
+        <v>176</v>
+      </c>
+      <c r="C6" s="53" t="s">
+        <v>177</v>
+      </c>
+      <c r="D6" s="53" t="s">
+        <v>174</v>
+      </c>
+      <c r="E6" s="55" t="s">
         <v>175</v>
-      </c>
-      <c r="C6" s="53" t="s">
-        <v>176</v>
-      </c>
-      <c r="D6" s="53" t="s">
-        <v>173</v>
-      </c>
-      <c r="E6" s="55" t="s">
-        <v>174</v>
       </c>
       <c r="F6" s="54"/>
       <c r="G6" s="54"/>
@@ -3123,17 +3124,17 @@
     </row>
     <row r="7" ht="27.75" customHeight="1">
       <c r="A7" s="47" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B7" s="48"/>
       <c r="C7" s="49" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D7" s="49" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E7" s="56" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F7" s="50"/>
       <c r="G7" s="50"/>
@@ -3156,16 +3157,16 @@
     </row>
     <row r="8" ht="27.75" customHeight="1">
       <c r="A8" s="51" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B8" s="57" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C8" s="58" t="s">
+        <v>169</v>
+      </c>
+      <c r="D8" s="58" t="s">
         <v>168</v>
-      </c>
-      <c r="D8" s="58" t="s">
-        <v>167</v>
       </c>
       <c r="E8" s="54"/>
       <c r="F8" s="54"/>
@@ -3189,14 +3190,14 @@
     </row>
     <row r="9" ht="27.75" customHeight="1">
       <c r="A9" s="47" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B9" s="48"/>
       <c r="C9" s="59" t="s">
+        <v>172</v>
+      </c>
+      <c r="D9" s="59" t="s">
         <v>171</v>
-      </c>
-      <c r="D9" s="59" t="s">
-        <v>170</v>
       </c>
       <c r="E9" s="50"/>
       <c r="F9" s="50"/>
@@ -3243,25 +3244,25 @@
   <sheetData>
     <row r="1" ht="23.25" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="36"/>
@@ -3287,7 +3288,7 @@
     </row>
     <row r="2" ht="23.25" customHeight="1">
       <c r="A2" s="60" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B2" s="2" t="str">
         <f t="shared" ref="B2:C2" si="1">"99.99"</f>
@@ -3307,10 +3308,10 @@
         <v>30.0</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H2" s="61" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="I2" s="36"/>
       <c r="J2" s="36"/>
@@ -3335,7 +3336,7 @@
     </row>
     <row r="3" ht="23.25" customHeight="1">
       <c r="A3" s="60" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B3" s="2" t="str">
         <f t="shared" ref="B3:C3" si="2">"999.99"</f>
@@ -3355,7 +3356,7 @@
         <v>50.0</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="H3" s="36"/>
       <c r="I3" s="36"/>
@@ -3381,7 +3382,7 @@
     </row>
     <row r="4" ht="23.25" customHeight="1">
       <c r="A4" s="60" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B4" s="2" t="str">
         <f t="shared" ref="B4:C4" si="3">"99999.99"</f>
@@ -3425,7 +3426,7 @@
     </row>
     <row r="5" ht="23.25" customHeight="1">
       <c r="A5" s="60" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B5" s="2" t="str">
         <f t="shared" ref="B5:C5" si="4">"99999.999"</f>
@@ -3469,7 +3470,7 @@
     </row>
     <row r="6" ht="23.25" customHeight="1">
       <c r="A6" s="60" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B6" s="2" t="str">
         <f t="shared" ref="B6:C6" si="5">"999999999.99"</f>
@@ -3513,7 +3514,7 @@
     </row>
     <row r="7" ht="23.25" customHeight="1">
       <c r="A7" s="60" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B7" s="2" t="str">
         <f t="shared" ref="B7:C7" si="6">"999999999.999"</f>
@@ -3557,7 +3558,7 @@
     </row>
     <row r="8" ht="23.25" customHeight="1">
       <c r="A8" s="60" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B8" s="2" t="str">
         <f t="shared" ref="B8:C8" si="7">"999999999999.999999"</f>
@@ -3601,7 +3602,7 @@
     </row>
     <row r="9" ht="23.25" customHeight="1">
       <c r="A9" s="60" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -3637,7 +3638,7 @@
     </row>
     <row r="10" ht="23.25" customHeight="1">
       <c r="A10" s="60" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B10" s="28"/>
       <c r="C10" s="2"/>
@@ -3673,7 +3674,7 @@
     </row>
     <row r="11" ht="23.25" customHeight="1">
       <c r="A11" s="60" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B11" s="28"/>
       <c r="C11" s="2"/>
@@ -3709,7 +3710,7 @@
     </row>
     <row r="12" ht="23.25" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B12" s="28"/>
       <c r="C12" s="2"/>
@@ -3745,7 +3746,7 @@
     </row>
     <row r="13" ht="23.25" customHeight="1">
       <c r="A13" s="60" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B13" s="28"/>
       <c r="C13" s="28"/>
@@ -3777,7 +3778,7 @@
     </row>
     <row r="14" ht="23.25" customHeight="1">
       <c r="A14" s="60" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B14" s="28"/>
       <c r="C14" s="28"/>
@@ -3809,7 +3810,7 @@
     </row>
     <row r="15" ht="23.25" customHeight="1">
       <c r="A15" s="60" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B15" s="28"/>
       <c r="C15" s="28"/>
@@ -3841,7 +3842,7 @@
     </row>
     <row r="16" ht="23.25" customHeight="1">
       <c r="A16" s="60" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" s="28"/>
       <c r="C16" s="28"/>
@@ -3873,7 +3874,7 @@
     </row>
     <row r="17" ht="23.25" customHeight="1">
       <c r="A17" s="60" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B17" s="28"/>
       <c r="C17" s="28"/>
@@ -3905,7 +3906,7 @@
     </row>
     <row r="18" ht="23.25" customHeight="1">
       <c r="A18" s="60" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B18" s="28"/>
       <c r="C18" s="28"/>
@@ -3937,7 +3938,7 @@
     </row>
     <row r="19" ht="23.25" customHeight="1">
       <c r="A19" s="60" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19" s="28"/>
       <c r="C19" s="28"/>
@@ -3969,7 +3970,7 @@
     </row>
     <row r="20" ht="23.25" customHeight="1">
       <c r="A20" s="60" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" s="28"/>
       <c r="C20" s="28"/>
@@ -4001,7 +4002,7 @@
     </row>
     <row r="21" ht="23.25" customHeight="1">
       <c r="A21" s="60" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B21" s="28"/>
       <c r="C21" s="28"/>
@@ -4033,7 +4034,7 @@
     </row>
     <row r="22" ht="23.25" customHeight="1">
       <c r="A22" s="62" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B22" s="28"/>
       <c r="C22" s="28"/>
@@ -4065,7 +4066,7 @@
     </row>
     <row r="23" ht="23.25" customHeight="1">
       <c r="A23" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B23" s="28"/>
       <c r="C23" s="28"/>
@@ -33468,16 +33469,16 @@
   <sheetData>
     <row r="1" ht="29.25" customHeight="1">
       <c r="A1" s="7" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="8"/>
@@ -33515,97 +33516,97 @@
     </row>
     <row r="3" ht="29.25" customHeight="1">
       <c r="A3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="D3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="E3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="F3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="G3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="H3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="I3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="J3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="K3" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="L3" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="M3" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="15" t="s">
+      <c r="N3" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="15" t="s">
+      <c r="O3" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="P3" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="P3" s="16" t="s">
+      <c r="Q3" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="Q3" s="16" t="s">
+      <c r="R3" s="16" t="s">
         <v>22</v>
-      </c>
-      <c r="R3" s="16" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="4" ht="29.25" customHeight="1">
       <c r="A4" s="26" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E4" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>26</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>27</v>
       </c>
       <c r="G4" s="29"/>
       <c r="H4" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I4" s="30"/>
       <c r="J4" s="31"/>
       <c r="K4" s="32"/>
       <c r="L4" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M4" s="9">
         <v>1.0</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P4" s="9"/>
       <c r="Q4" s="9"/>
@@ -33670,13 +33671,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="7" t="s">
         <v>4</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>5</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="8"/>
@@ -33715,175 +33716,175 @@
     </row>
     <row r="3" ht="29.25" customHeight="1">
       <c r="A3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="D3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="E3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="F3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="G3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="H3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="I3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="J3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="K3" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="L3" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="M3" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="15" t="s">
+      <c r="N3" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="15" t="s">
+      <c r="O3" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="P3" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="P3" s="16" t="s">
+      <c r="Q3" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="Q3" s="16" t="s">
+      <c r="R3" s="16" t="s">
         <v>22</v>
-      </c>
-      <c r="R3" s="16" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="4" ht="29.25" customHeight="1">
       <c r="A4" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="18" t="s">
-        <v>25</v>
-      </c>
       <c r="C4" s="18" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" s="18"/>
       <c r="E4" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="19" t="s">
         <v>26</v>
-      </c>
-      <c r="F4" s="19" t="s">
-        <v>27</v>
       </c>
       <c r="G4" s="20"/>
       <c r="H4" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I4" s="21"/>
       <c r="J4" s="21"/>
       <c r="K4" s="22"/>
       <c r="L4" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M4" s="19"/>
       <c r="N4" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O4" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P4" s="19"/>
       <c r="Q4" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R4" s="24"/>
     </row>
     <row r="5" ht="29.25" customHeight="1">
       <c r="A5" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="18" t="s">
-        <v>31</v>
-      </c>
       <c r="C5" s="18" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5" s="18"/>
       <c r="E5" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5" s="23">
         <v>50.0</v>
       </c>
       <c r="G5" s="20"/>
       <c r="H5" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I5" s="21"/>
       <c r="J5" s="21"/>
       <c r="K5" s="22"/>
       <c r="L5" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M5" s="18">
         <v>1.0</v>
       </c>
       <c r="N5" s="25"/>
       <c r="O5" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P5" s="18">
         <v>1.0</v>
       </c>
       <c r="Q5" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R5" s="24"/>
     </row>
     <row r="6" ht="29.25" customHeight="1">
       <c r="A6" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="18" t="s">
-        <v>34</v>
-      </c>
       <c r="C6" s="18" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F6" s="23">
         <v>50.0</v>
       </c>
       <c r="G6" s="20"/>
       <c r="H6" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I6" s="21"/>
       <c r="J6" s="21"/>
       <c r="K6" s="22"/>
       <c r="L6" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M6" s="18">
         <v>2.0</v>
       </c>
       <c r="N6" s="25"/>
       <c r="O6" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P6" s="25"/>
       <c r="Q6" s="9"/>
@@ -33891,20 +33892,20 @@
     </row>
     <row r="7" ht="29.25" customHeight="1">
       <c r="A7" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="18" t="s">
-        <v>36</v>
-      </c>
       <c r="C7" s="18" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G7" s="20"/>
       <c r="H7" s="19"/>
@@ -33912,12 +33913,12 @@
       <c r="J7" s="21"/>
       <c r="K7" s="22"/>
       <c r="L7" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M7" s="18"/>
       <c r="N7" s="25"/>
       <c r="O7" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P7" s="25"/>
       <c r="Q7" s="9"/>
@@ -33925,35 +33926,35 @@
     </row>
     <row r="8" ht="29.25" customHeight="1">
       <c r="A8" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="C8" s="18" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F8" s="23">
         <v>50.0</v>
       </c>
       <c r="G8" s="20"/>
       <c r="H8" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I8" s="21"/>
       <c r="J8" s="21"/>
       <c r="K8" s="22"/>
       <c r="L8" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M8" s="18"/>
       <c r="N8" s="25"/>
       <c r="O8" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P8" s="25"/>
       <c r="Q8" s="9"/>
@@ -33961,36 +33962,36 @@
     </row>
     <row r="9" ht="29.25" customHeight="1">
       <c r="A9" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="18" t="s">
-        <v>41</v>
-      </c>
       <c r="C9" s="18" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9" s="18"/>
       <c r="E9" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F9" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="23" t="s">
         <v>27</v>
-      </c>
-      <c r="G9" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="H9" s="23" t="s">
-        <v>28</v>
       </c>
       <c r="I9" s="21"/>
       <c r="J9" s="21"/>
       <c r="K9" s="22"/>
       <c r="L9" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M9" s="18"/>
       <c r="N9" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O9" s="25"/>
       <c r="P9" s="25"/>
@@ -33999,36 +34000,36 @@
     </row>
     <row r="10" ht="29.25" customHeight="1">
       <c r="A10" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="18" t="s">
-        <v>44</v>
-      </c>
       <c r="C10" s="18" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D10" s="18"/>
       <c r="E10" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="23" t="s">
+      <c r="H10" s="23" t="s">
         <v>27</v>
-      </c>
-      <c r="G10" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="H10" s="23" t="s">
-        <v>28</v>
       </c>
       <c r="I10" s="21"/>
       <c r="J10" s="21"/>
       <c r="K10" s="22"/>
       <c r="L10" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M10" s="18"/>
       <c r="N10" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O10" s="25"/>
       <c r="P10" s="25"/>
@@ -34102,13 +34103,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>46</v>
-      </c>
       <c r="D1" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="8"/>
@@ -34147,95 +34148,95 @@
     </row>
     <row r="3" ht="29.25" customHeight="1">
       <c r="A3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="D3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="E3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="F3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="G3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="H3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="I3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="J3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="K3" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="L3" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="M3" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="15" t="s">
+      <c r="N3" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="15" t="s">
+      <c r="O3" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="P3" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="P3" s="16" t="s">
+      <c r="Q3" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="Q3" s="16" t="s">
+      <c r="R3" s="16" t="s">
         <v>22</v>
-      </c>
-      <c r="R3" s="16" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="4" ht="29.25" customHeight="1">
       <c r="A4" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E4" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>26</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>27</v>
       </c>
       <c r="G4" s="29"/>
       <c r="H4" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I4" s="30"/>
       <c r="J4" s="31"/>
       <c r="K4" s="32"/>
       <c r="L4" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M4" s="9"/>
       <c r="N4" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P4" s="9"/>
       <c r="Q4" s="9"/>
@@ -34243,41 +34244,41 @@
     </row>
     <row r="5" ht="29.25" customHeight="1">
       <c r="A5" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5" s="9">
         <v>50.0</v>
       </c>
       <c r="G5" s="29"/>
       <c r="H5" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I5" s="30"/>
       <c r="J5" s="31"/>
       <c r="K5" s="32"/>
       <c r="L5" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M5" s="9">
         <v>1.0</v>
       </c>
       <c r="N5" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O5" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P5" s="9">
         <v>1.0</v>
@@ -34287,43 +34288,43 @@
     </row>
     <row r="6" ht="29.25" customHeight="1">
       <c r="A6" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" s="9" t="s">
+      <c r="H6" s="9" t="s">
         <v>27</v>
-      </c>
-      <c r="G6" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>28</v>
       </c>
       <c r="I6" s="30"/>
       <c r="J6" s="31"/>
       <c r="K6" s="32"/>
       <c r="L6" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M6" s="9">
         <v>2.0</v>
       </c>
       <c r="N6" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="O6" s="18" t="s">
         <v>28</v>
-      </c>
-      <c r="O6" s="18" t="s">
-        <v>29</v>
       </c>
       <c r="P6" s="9"/>
       <c r="Q6" s="9"/>
@@ -34331,37 +34332,37 @@
     </row>
     <row r="7" ht="29.25" customHeight="1">
       <c r="A7" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>56</v>
-      </c>
       <c r="F7" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G7" s="29"/>
       <c r="H7" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I7" s="30"/>
       <c r="J7" s="31"/>
       <c r="K7" s="32"/>
       <c r="L7" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M7" s="9"/>
       <c r="N7" s="9"/>
       <c r="O7" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P7" s="9"/>
       <c r="Q7" s="9"/>
@@ -34371,37 +34372,37 @@
     </row>
     <row r="8" ht="29.25" customHeight="1">
       <c r="A8" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="E8" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F8" s="9">
         <v>50.0</v>
       </c>
       <c r="G8" s="29"/>
       <c r="H8" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I8" s="30"/>
       <c r="J8" s="31"/>
       <c r="K8" s="32"/>
       <c r="L8" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M8" s="9"/>
       <c r="N8" s="9"/>
       <c r="O8" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P8" s="9"/>
       <c r="Q8" s="9"/>
@@ -34409,37 +34410,37 @@
     </row>
     <row r="9" ht="29.25" customHeight="1">
       <c r="A9" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="C9" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F9" s="9">
         <v>50.0</v>
       </c>
       <c r="G9" s="29"/>
       <c r="H9" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I9" s="30"/>
       <c r="J9" s="31"/>
       <c r="K9" s="32"/>
       <c r="L9" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M9" s="9"/>
       <c r="N9" s="9"/>
       <c r="O9" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P9" s="9"/>
       <c r="Q9" s="9"/>
@@ -34447,37 +34448,37 @@
     </row>
     <row r="10" ht="29.25" customHeight="1">
       <c r="A10" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="C10" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F10" s="9">
         <v>50.0</v>
       </c>
       <c r="G10" s="29"/>
       <c r="H10" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I10" s="30"/>
       <c r="J10" s="31"/>
       <c r="K10" s="32"/>
       <c r="L10" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M10" s="9"/>
       <c r="N10" s="9"/>
       <c r="O10" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P10" s="9"/>
       <c r="Q10" s="9"/>
@@ -34485,37 +34486,37 @@
     </row>
     <row r="11" ht="29.25" customHeight="1">
       <c r="A11" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="C11" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F11" s="9">
         <v>50.0</v>
       </c>
       <c r="G11" s="29"/>
       <c r="H11" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I11" s="30"/>
       <c r="J11" s="31"/>
       <c r="K11" s="32"/>
       <c r="L11" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M11" s="9"/>
       <c r="N11" s="9"/>
       <c r="O11" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P11" s="9"/>
       <c r="Q11" s="9"/>
@@ -34523,37 +34524,37 @@
     </row>
     <row r="12" ht="29.25" customHeight="1">
       <c r="A12" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>68</v>
-      </c>
       <c r="F12" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G12" s="29"/>
       <c r="H12" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I12" s="30"/>
       <c r="J12" s="31"/>
       <c r="K12" s="32"/>
       <c r="L12" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M12" s="9"/>
       <c r="N12" s="9"/>
       <c r="O12" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P12" s="9"/>
       <c r="Q12" s="9"/>
@@ -34561,26 +34562,24 @@
     </row>
     <row r="13" ht="29.25" customHeight="1">
       <c r="A13" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="C13" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G13" s="29" t="s">
-        <v>72</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="G13" s="29"/>
       <c r="H13" s="9" t="s">
         <v>28</v>
       </c>
@@ -34588,14 +34587,12 @@
       <c r="J13" s="31"/>
       <c r="K13" s="32"/>
       <c r="L13" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="18" t="s">
         <v>28</v>
-      </c>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="O13" s="18" t="s">
-        <v>29</v>
       </c>
       <c r="P13" s="9"/>
       <c r="Q13" s="9"/>
@@ -34603,41 +34600,41 @@
     </row>
     <row r="14" ht="29.25" customHeight="1">
       <c r="A14" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="F14" s="9" t="s">
+      <c r="H14" s="9" t="s">
         <v>27</v>
-      </c>
-      <c r="G14" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>29</v>
       </c>
       <c r="I14" s="30"/>
       <c r="J14" s="31"/>
       <c r="K14" s="32"/>
       <c r="L14" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M14" s="9"/>
       <c r="N14" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="O14" s="18" t="s">
         <v>28</v>
-      </c>
-      <c r="O14" s="18" t="s">
-        <v>29</v>
       </c>
       <c r="P14" s="9"/>
       <c r="Q14" s="9"/>
@@ -34645,24 +34642,26 @@
     </row>
     <row r="15" ht="29.25" customHeight="1">
       <c r="A15" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="F15" s="9">
-        <v>999.0</v>
-      </c>
-      <c r="G15" s="29"/>
       <c r="H15" s="9" t="s">
         <v>28</v>
       </c>
@@ -34670,10 +34669,12 @@
       <c r="J15" s="31"/>
       <c r="K15" s="32"/>
       <c r="L15" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
+      <c r="N15" s="9" t="s">
+        <v>27</v>
+      </c>
       <c r="O15" s="18" t="s">
         <v>28</v>
       </c>
@@ -34682,164 +34683,202 @@
       <c r="R15" s="9"/>
     </row>
     <row r="16" ht="29.25" customHeight="1">
-      <c r="A16" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="18" t="s">
+      <c r="A16" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E16" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E16" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="F16" s="23">
-        <v>50.0</v>
-      </c>
-      <c r="G16" s="18"/>
+      <c r="F16" s="9">
+        <v>999.0</v>
+      </c>
+      <c r="G16" s="29"/>
       <c r="H16" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="22"/>
+        <v>27</v>
+      </c>
+      <c r="I16" s="30"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="32"/>
       <c r="L16" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="M16" s="18"/>
-      <c r="N16" s="18"/>
+        <v>27</v>
+      </c>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
       <c r="O16" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="P16" s="20"/>
+        <v>27</v>
+      </c>
+      <c r="P16" s="9"/>
       <c r="Q16" s="9"/>
-      <c r="R16" s="24"/>
+      <c r="R16" s="9"/>
     </row>
     <row r="17" ht="29.25" customHeight="1">
       <c r="A17" s="17" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="F17" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" s="23">
+        <v>50.0</v>
+      </c>
+      <c r="G17" s="18"/>
+      <c r="H17" s="9" t="s">
         <v>27</v>
-      </c>
-      <c r="G17" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="H17" s="9" t="s">
-        <v>28</v>
       </c>
       <c r="I17" s="21"/>
       <c r="J17" s="21"/>
       <c r="K17" s="22"/>
       <c r="L17" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M17" s="18"/>
-      <c r="N17" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="O17" s="20"/>
+      <c r="N17" s="18"/>
+      <c r="O17" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="P17" s="20"/>
       <c r="Q17" s="9"/>
       <c r="R17" s="24"/>
     </row>
     <row r="18" ht="29.25" customHeight="1">
       <c r="A18" s="17" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B18" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="D18" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E18" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F18" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="H18" s="9" t="s">
         <v>27</v>
-      </c>
-      <c r="G18" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="H18" s="23" t="s">
-        <v>28</v>
       </c>
       <c r="I18" s="21"/>
       <c r="J18" s="21"/>
       <c r="K18" s="22"/>
       <c r="L18" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M18" s="18"/>
       <c r="N18" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O18" s="20"/>
       <c r="P18" s="20"/>
       <c r="Q18" s="9"/>
       <c r="R18" s="24"/>
     </row>
+    <row r="19" ht="29.25" customHeight="1">
+      <c r="A19" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="H19" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="22"/>
+      <c r="L19" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="M19" s="18"/>
+      <c r="N19" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="O19" s="20"/>
+      <c r="P19" s="20"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="24"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="R16:R18">
+  <conditionalFormatting sqref="R17:R19">
     <cfRule type="containsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(R16))=0</formula>
+      <formula>LEN(TRIM(R17))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please select the table you want for the field." sqref="G13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please select the table you want for the field." sqref="G14">
       <formula1>"Reagent,Plasmids,Enzyme,Primer,Antibody,Supplier,EnzymeType,VectorType,GrowthStrains,AntibioticResistance,Lab"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please select the format you want for the field." sqref="F5 F8:F11 F16">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please select the format you want for the field." sqref="F5 F8:F11 F17">
       <formula1>"30,50,100,130,150,200,255,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Please select the application to which this table should be associated to." sqref="A1">
       <formula1>Applications!$A$2:$A$16</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please select a field to which this field depends on to be visible." sqref="I4:I19">
-      <formula1>Table_Plasmids!$B$4:$B$18</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please select the table you want for the field." sqref="G14">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please select the table you want for the field." sqref="G15">
       <formula1>"Reagent,Plasmids,Enzyme,Primer,Antibody,Supplier,EnzymeType,VectorType,GrowthStrains,Lab"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E4:E15">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E4:E16">
       <formula1>Configurations!$A$1:$A$30</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Set the type of data access you want for this table" sqref="D1">
       <formula1>"All data is accessible to users,Restrict data access by the creator,Restrict data access by the creator group"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please select the table you want for the field." sqref="G17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please select a field to which this field depends on to be visible." sqref="I4:I20">
+      <formula1>Table_Plasmids!$B$4:$B$19</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please select the table you want for the field." sqref="G18">
       <formula1>"Reagent,Supplier,Lab"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please select the format you want for the field." sqref="F15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please select the format you want for the field." sqref="F16">
       <formula1>"9,99,999,9999,99999,999999,9999999,99999999,999999999,9999999999,999999999999,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E16:E18">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E17:E19">
       <formula1>Configurations!$A$2:$A$30</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please select the table you want for the field." sqref="G18">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please select the table you want for the field." sqref="G19">
       <formula1>"Reagent,Lab"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="H4:H18 L4:L18 N4:O18 Q4:Q18">
+    <dataValidation type="list" allowBlank="1" sqref="H4:H19 L4:L19 N4:O19 Q4:Q19">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please select the table you want for the field." sqref="G6">
@@ -34881,13 +34920,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="8"/>
@@ -34926,93 +34965,93 @@
     </row>
     <row r="3" ht="29.25" customHeight="1">
       <c r="A3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="D3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="E3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="F3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="G3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="H3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="I3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="J3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="K3" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="L3" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="M3" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="15" t="s">
+      <c r="N3" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="15" t="s">
+      <c r="O3" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="P3" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="P3" s="16" t="s">
+      <c r="Q3" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="Q3" s="16" t="s">
+      <c r="R3" s="16" t="s">
         <v>22</v>
-      </c>
-      <c r="R3" s="16" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="4" ht="29.25" customHeight="1">
       <c r="A4" s="26" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>26</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>27</v>
       </c>
       <c r="G4" s="29"/>
       <c r="H4" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I4" s="30"/>
       <c r="J4" s="31"/>
       <c r="K4" s="32"/>
       <c r="L4" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M4" s="9"/>
       <c r="N4" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P4" s="9"/>
       <c r="Q4" s="9"/>
@@ -35020,30 +35059,30 @@
     </row>
     <row r="5" ht="29.25" customHeight="1">
       <c r="A5" s="26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5" s="9">
         <v>50.0</v>
       </c>
       <c r="G5" s="29"/>
       <c r="H5" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I5" s="30"/>
       <c r="J5" s="31"/>
       <c r="K5" s="32"/>
       <c r="L5" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M5" s="9">
         <v>1.0</v>
@@ -35056,35 +35095,35 @@
     </row>
     <row r="6" ht="29.25" customHeight="1">
       <c r="A6" s="26" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D6" s="28"/>
       <c r="E6" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G6" s="28"/>
       <c r="H6" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I6" s="28"/>
       <c r="J6" s="28"/>
       <c r="K6" s="28"/>
       <c r="L6" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M6" s="28"/>
       <c r="N6" s="28"/>
       <c r="O6" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P6" s="28"/>
       <c r="Q6" s="28"/>
@@ -35092,35 +35131,35 @@
     </row>
     <row r="7" ht="29.25" customHeight="1">
       <c r="A7" s="26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F7" s="23">
         <v>50.0</v>
       </c>
       <c r="G7" s="20"/>
       <c r="H7" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I7" s="21"/>
       <c r="J7" s="21"/>
       <c r="K7" s="22"/>
       <c r="L7" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M7" s="18"/>
       <c r="N7" s="25"/>
       <c r="O7" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P7" s="25"/>
       <c r="Q7" s="9"/>
@@ -35128,38 +35167,38 @@
     </row>
     <row r="8" ht="29.25" customHeight="1">
       <c r="A8" s="26" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F8" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="H8" s="23" t="s">
         <v>27</v>
-      </c>
-      <c r="G8" s="29" t="s">
-        <v>91</v>
-      </c>
-      <c r="H8" s="23" t="s">
-        <v>28</v>
       </c>
       <c r="I8" s="30"/>
       <c r="J8" s="31"/>
       <c r="K8" s="32"/>
       <c r="L8" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M8" s="9">
         <v>2.0</v>
       </c>
       <c r="N8" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O8" s="9"/>
       <c r="P8" s="9"/>
@@ -35168,36 +35207,36 @@
     </row>
     <row r="9" ht="29.25" customHeight="1">
       <c r="A9" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="18" t="s">
-        <v>41</v>
-      </c>
       <c r="C9" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D9" s="18"/>
       <c r="E9" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F9" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="23" t="s">
         <v>27</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="H9" s="23" t="s">
-        <v>28</v>
       </c>
       <c r="I9" s="21"/>
       <c r="J9" s="21"/>
       <c r="K9" s="22"/>
       <c r="L9" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M9" s="18"/>
       <c r="N9" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O9" s="20"/>
       <c r="P9" s="20"/>
@@ -35206,36 +35245,36 @@
     </row>
     <row r="10" ht="29.25" customHeight="1">
       <c r="A10" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="18" t="s">
-        <v>44</v>
-      </c>
       <c r="C10" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D10" s="18"/>
       <c r="E10" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="23" t="s">
+      <c r="H10" s="23" t="s">
         <v>27</v>
-      </c>
-      <c r="G10" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="H10" s="23" t="s">
-        <v>28</v>
       </c>
       <c r="I10" s="21"/>
       <c r="J10" s="21"/>
       <c r="K10" s="22"/>
       <c r="L10" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M10" s="18"/>
       <c r="N10" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O10" s="20"/>
       <c r="P10" s="20"/>
@@ -35315,13 +35354,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="8"/>
@@ -35359,93 +35398,93 @@
     </row>
     <row r="3" ht="29.25" customHeight="1">
       <c r="A3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="D3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="E3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="F3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="G3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="H3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="I3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="J3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="K3" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="L3" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="M3" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="15" t="s">
+      <c r="N3" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="15" t="s">
+      <c r="O3" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="P3" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="P3" s="16" t="s">
+      <c r="Q3" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="Q3" s="16" t="s">
+      <c r="R3" s="16" t="s">
         <v>22</v>
-      </c>
-      <c r="R3" s="16" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="4" ht="29.25" customHeight="1">
       <c r="A4" s="26" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D4" s="33"/>
       <c r="E4" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>26</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>27</v>
       </c>
       <c r="G4" s="29"/>
       <c r="H4" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I4" s="30"/>
       <c r="J4" s="31"/>
       <c r="K4" s="32"/>
       <c r="L4" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M4" s="9"/>
       <c r="N4" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P4" s="9"/>
       <c r="Q4" s="9"/>
@@ -35453,37 +35492,37 @@
     </row>
     <row r="5" ht="29.25" customHeight="1">
       <c r="A5" s="17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5" s="23">
         <v>50.0</v>
       </c>
       <c r="G5" s="20"/>
       <c r="H5" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I5" s="21"/>
       <c r="J5" s="21"/>
       <c r="K5" s="22"/>
       <c r="L5" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M5" s="18">
         <v>1.0</v>
       </c>
       <c r="N5" s="25"/>
       <c r="O5" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P5" s="18">
         <v>1.0</v>
@@ -35493,37 +35532,37 @@
     </row>
     <row r="6" ht="29.25" customHeight="1">
       <c r="A6" s="26" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D6" s="33"/>
       <c r="E6" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F6" s="9">
         <v>100.0</v>
       </c>
       <c r="G6" s="29"/>
       <c r="H6" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I6" s="30"/>
       <c r="J6" s="31"/>
       <c r="K6" s="32"/>
       <c r="L6" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M6" s="9">
         <v>2.0</v>
       </c>
       <c r="N6" s="9"/>
       <c r="O6" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P6" s="9"/>
       <c r="Q6" s="9"/>
@@ -35531,35 +35570,35 @@
     </row>
     <row r="7" ht="29.25" customHeight="1">
       <c r="A7" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G7" s="20"/>
       <c r="H7" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I7" s="21"/>
       <c r="J7" s="21"/>
       <c r="K7" s="22"/>
       <c r="L7" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M7" s="18"/>
       <c r="N7" s="25"/>
       <c r="O7" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P7" s="25"/>
       <c r="Q7" s="9"/>
@@ -35567,35 +35606,35 @@
     </row>
     <row r="8" ht="29.25" customHeight="1">
       <c r="A8" s="17" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="23" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F8" s="23">
         <v>999.0</v>
       </c>
       <c r="G8" s="20"/>
       <c r="H8" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I8" s="21"/>
       <c r="J8" s="21"/>
       <c r="K8" s="22"/>
       <c r="L8" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M8" s="18"/>
       <c r="N8" s="25"/>
       <c r="O8" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P8" s="25"/>
       <c r="Q8" s="9"/>
@@ -35603,36 +35642,36 @@
     </row>
     <row r="9" ht="29.25" customHeight="1">
       <c r="A9" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="18" t="s">
-        <v>44</v>
-      </c>
       <c r="C9" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="F9" s="23" t="s">
+      <c r="H9" s="23" t="s">
         <v>27</v>
-      </c>
-      <c r="G9" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="H9" s="23" t="s">
-        <v>28</v>
       </c>
       <c r="I9" s="21"/>
       <c r="J9" s="21"/>
       <c r="K9" s="22"/>
       <c r="L9" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M9" s="18"/>
       <c r="N9" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O9" s="25"/>
       <c r="P9" s="25"/>
@@ -35641,36 +35680,36 @@
     </row>
     <row r="10" ht="29.25" customHeight="1">
       <c r="A10" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="18" t="s">
-        <v>41</v>
-      </c>
       <c r="C10" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F10" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10" s="23" t="s">
         <v>27</v>
-      </c>
-      <c r="G10" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="H10" s="23" t="s">
-        <v>28</v>
       </c>
       <c r="I10" s="21"/>
       <c r="J10" s="21"/>
       <c r="K10" s="22"/>
       <c r="L10" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M10" s="18"/>
       <c r="N10" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O10" s="25"/>
       <c r="P10" s="25"/>
@@ -35750,13 +35789,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="8"/>
@@ -35794,93 +35833,93 @@
     </row>
     <row r="3" ht="29.25" customHeight="1">
       <c r="A3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="D3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="E3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="F3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="G3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="H3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="I3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="J3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="K3" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="L3" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="M3" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="15" t="s">
+      <c r="N3" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="15" t="s">
+      <c r="O3" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="P3" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="P3" s="16" t="s">
+      <c r="Q3" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="Q3" s="16" t="s">
+      <c r="R3" s="16" t="s">
         <v>22</v>
-      </c>
-      <c r="R3" s="16" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="4" ht="29.25" customHeight="1">
       <c r="A4" s="26" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>26</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>27</v>
       </c>
       <c r="G4" s="29"/>
       <c r="H4" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I4" s="30"/>
       <c r="J4" s="31"/>
       <c r="K4" s="32"/>
       <c r="L4" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M4" s="9"/>
       <c r="N4" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P4" s="9"/>
       <c r="Q4" s="9"/>
@@ -35888,37 +35927,37 @@
     </row>
     <row r="5" ht="29.25" customHeight="1">
       <c r="A5" s="26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5" s="23">
         <v>50.0</v>
       </c>
       <c r="G5" s="20"/>
       <c r="H5" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I5" s="21"/>
       <c r="J5" s="21"/>
       <c r="K5" s="22"/>
       <c r="L5" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M5" s="18">
         <v>1.0</v>
       </c>
       <c r="N5" s="25"/>
       <c r="O5" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P5" s="18">
         <v>1.0</v>
@@ -35928,37 +35967,37 @@
     </row>
     <row r="6" ht="29.25" customHeight="1">
       <c r="A6" s="26" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F6" s="23">
         <v>50.0</v>
       </c>
       <c r="G6" s="20"/>
       <c r="H6" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I6" s="21"/>
       <c r="J6" s="21"/>
       <c r="K6" s="22"/>
       <c r="L6" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M6" s="18">
         <v>2.0</v>
       </c>
       <c r="N6" s="25"/>
       <c r="O6" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P6" s="25"/>
       <c r="Q6" s="9"/>
@@ -35966,35 +36005,35 @@
     </row>
     <row r="7" ht="29.25" customHeight="1">
       <c r="A7" s="26" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F7" s="23">
         <v>50.0</v>
       </c>
       <c r="G7" s="20"/>
       <c r="H7" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I7" s="21"/>
       <c r="J7" s="21"/>
       <c r="K7" s="22"/>
       <c r="L7" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M7" s="18"/>
       <c r="N7" s="25"/>
       <c r="O7" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P7" s="25"/>
       <c r="Q7" s="9"/>
@@ -36002,35 +36041,35 @@
     </row>
     <row r="8" ht="29.25" customHeight="1">
       <c r="A8" s="26" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F8" s="23">
         <v>50.0</v>
       </c>
       <c r="G8" s="20"/>
       <c r="H8" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I8" s="21"/>
       <c r="J8" s="21"/>
       <c r="K8" s="22"/>
       <c r="L8" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M8" s="18"/>
       <c r="N8" s="25"/>
       <c r="O8" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P8" s="25"/>
       <c r="Q8" s="9"/>
@@ -36038,35 +36077,35 @@
     </row>
     <row r="9" ht="29.25" customHeight="1">
       <c r="A9" s="26" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F9" s="23">
         <v>50.0</v>
       </c>
       <c r="G9" s="20"/>
       <c r="H9" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I9" s="21"/>
       <c r="J9" s="21"/>
       <c r="K9" s="22"/>
       <c r="L9" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M9" s="18"/>
       <c r="N9" s="25"/>
       <c r="O9" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P9" s="25"/>
       <c r="Q9" s="9"/>
@@ -36074,35 +36113,35 @@
     </row>
     <row r="10" ht="29.25" customHeight="1">
       <c r="A10" s="26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F10" s="23">
         <v>50.0</v>
       </c>
       <c r="G10" s="20"/>
       <c r="H10" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I10" s="21"/>
       <c r="J10" s="21"/>
       <c r="K10" s="22"/>
       <c r="L10" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M10" s="18"/>
       <c r="N10" s="25"/>
       <c r="O10" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P10" s="25"/>
       <c r="Q10" s="9"/>
@@ -36110,35 +36149,35 @@
     </row>
     <row r="11" ht="29.25" customHeight="1">
       <c r="A11" s="17" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D11" s="18"/>
       <c r="E11" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F11" s="23">
         <v>50.0</v>
       </c>
       <c r="G11" s="27"/>
       <c r="H11" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I11" s="21"/>
       <c r="J11" s="21"/>
       <c r="K11" s="22"/>
       <c r="L11" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M11" s="18"/>
       <c r="N11" s="18"/>
       <c r="O11" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P11" s="25"/>
       <c r="Q11" s="9"/>
@@ -36149,32 +36188,32 @@
         <v>0</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D12" s="18"/>
       <c r="E12" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F12" s="23">
         <v>50.0</v>
       </c>
       <c r="G12" s="27"/>
       <c r="H12" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I12" s="21"/>
       <c r="J12" s="21"/>
       <c r="K12" s="22"/>
       <c r="L12" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M12" s="18"/>
       <c r="N12" s="18"/>
       <c r="O12" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P12" s="25"/>
       <c r="Q12" s="9"/>
@@ -36182,36 +36221,36 @@
     </row>
     <row r="13" ht="29.25" customHeight="1">
       <c r="A13" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="18" t="s">
-        <v>41</v>
-      </c>
       <c r="C13" s="18" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D13" s="18"/>
       <c r="E13" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F13" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="H13" s="23" t="s">
         <v>27</v>
-      </c>
-      <c r="G13" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="H13" s="23" t="s">
-        <v>28</v>
       </c>
       <c r="I13" s="21"/>
       <c r="J13" s="21"/>
       <c r="K13" s="22"/>
       <c r="L13" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M13" s="18"/>
       <c r="N13" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O13" s="25"/>
       <c r="P13" s="25"/>
@@ -36285,13 +36324,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="8"/>
@@ -36329,95 +36368,95 @@
     </row>
     <row r="3" ht="29.25" customHeight="1">
       <c r="A3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="D3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="E3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="F3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="G3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="H3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="I3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="J3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="K3" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="L3" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="M3" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="15" t="s">
+      <c r="N3" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="15" t="s">
+      <c r="O3" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="P3" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="P3" s="16" t="s">
+      <c r="Q3" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="Q3" s="16" t="s">
+      <c r="R3" s="16" t="s">
         <v>22</v>
-      </c>
-      <c r="R3" s="16" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="4" ht="29.25" customHeight="1">
       <c r="A4" s="26" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>26</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>27</v>
       </c>
       <c r="G4" s="29"/>
       <c r="H4" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I4" s="30"/>
       <c r="J4" s="31"/>
       <c r="K4" s="32"/>
       <c r="L4" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M4" s="9">
         <v>1.0</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P4" s="9"/>
       <c r="Q4" s="9"/>
@@ -36425,45 +36464,45 @@
     </row>
     <row r="5" ht="29.25" customHeight="1">
       <c r="A5" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>121</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5" s="9">
         <v>100.0</v>
       </c>
       <c r="G5" s="29"/>
       <c r="H5" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I5" s="30"/>
       <c r="J5" s="31"/>
       <c r="K5" s="32"/>
       <c r="L5" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M5" s="9">
         <v>2.0</v>
       </c>
       <c r="N5" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P5" s="9">
         <v>1.0</v>
       </c>
       <c r="Q5" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R5" s="9"/>
     </row>
@@ -36523,13 +36562,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="8"/>
@@ -36567,95 +36606,95 @@
     </row>
     <row r="3" ht="29.25" customHeight="1">
       <c r="A3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="D3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="E3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="F3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="G3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="H3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="I3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="J3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="K3" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="L3" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="M3" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="15" t="s">
+      <c r="N3" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="15" t="s">
+      <c r="O3" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="P3" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="P3" s="16" t="s">
+      <c r="Q3" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="Q3" s="16" t="s">
+      <c r="R3" s="16" t="s">
         <v>22</v>
-      </c>
-      <c r="R3" s="16" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="4" ht="29.25" customHeight="1">
       <c r="A4" s="26" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>26</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>27</v>
       </c>
       <c r="G4" s="29"/>
       <c r="H4" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I4" s="30"/>
       <c r="J4" s="31"/>
       <c r="K4" s="32"/>
       <c r="L4" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M4" s="9">
         <v>1.0</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P4" s="9"/>
       <c r="Q4" s="9"/>
@@ -36663,45 +36702,45 @@
     </row>
     <row r="5" ht="29.25" customHeight="1">
       <c r="A5" s="26" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5" s="9">
         <v>100.0</v>
       </c>
       <c r="G5" s="29"/>
       <c r="H5" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I5" s="30"/>
       <c r="J5" s="31"/>
       <c r="K5" s="32"/>
       <c r="L5" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M5" s="9">
         <v>2.0</v>
       </c>
       <c r="N5" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P5" s="9">
         <v>1.0</v>
       </c>
       <c r="Q5" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R5" s="9"/>
     </row>
@@ -36761,13 +36800,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="8"/>
@@ -36805,95 +36844,95 @@
     </row>
     <row r="3" ht="29.25" customHeight="1">
       <c r="A3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="D3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="E3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="F3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="G3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="H3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="I3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="J3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="K3" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="L3" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="M3" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="15" t="s">
+      <c r="N3" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="15" t="s">
+      <c r="O3" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="P3" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="P3" s="16" t="s">
+      <c r="Q3" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="Q3" s="16" t="s">
+      <c r="R3" s="16" t="s">
         <v>22</v>
-      </c>
-      <c r="R3" s="16" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="4" ht="29.25" customHeight="1">
       <c r="A4" s="26" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>26</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>27</v>
       </c>
       <c r="G4" s="29"/>
       <c r="H4" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I4" s="30"/>
       <c r="J4" s="31"/>
       <c r="K4" s="32"/>
       <c r="L4" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M4" s="9">
         <v>1.0</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P4" s="9"/>
       <c r="Q4" s="9"/>
@@ -36901,45 +36940,45 @@
     </row>
     <row r="5" ht="29.25" customHeight="1">
       <c r="A5" s="26" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5" s="9">
         <v>100.0</v>
       </c>
       <c r="G5" s="29"/>
       <c r="H5" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I5" s="30"/>
       <c r="J5" s="31"/>
       <c r="K5" s="32"/>
       <c r="L5" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M5" s="9">
         <v>2.0</v>
       </c>
       <c r="N5" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P5" s="9">
         <v>1.0</v>
       </c>
       <c r="Q5" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R5" s="9"/>
     </row>

</xml_diff>